<commit_message>
fix tid, lav løsning
</commit_message>
<xml_diff>
--- a/VL.xlsx
+++ b/VL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebk\makro\p6_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB86992-F792-49D6-A974-BC5E2BD4C5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6414DC86-9DF9-405B-A940-125D19FD324A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="3360" windowWidth="21600" windowHeight="10785" xr2:uid="{E7DE5B6D-17B1-4BBB-8342-C7DA09B36074}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="56">
   <si>
     <t>24-2267</t>
   </si>
@@ -174,10 +174,37 @@
     <t>fv8</t>
   </si>
   <si>
-    <t>18:00</t>
-  </si>
-  <si>
     <t>16:55</t>
+  </si>
+  <si>
+    <t>16:52</t>
+  </si>
+  <si>
+    <t>18:02</t>
+  </si>
+  <si>
+    <t>16:53</t>
+  </si>
+  <si>
+    <t>18:03</t>
+  </si>
+  <si>
+    <t>16:54</t>
+  </si>
+  <si>
+    <t>18:04</t>
+  </si>
+  <si>
+    <t>16:51</t>
+  </si>
+  <si>
+    <t>18:01</t>
+  </si>
+  <si>
+    <t>16:56</t>
+  </si>
+  <si>
+    <t>18:05</t>
   </si>
 </sst>
 </file>
@@ -587,7 +614,7 @@
   <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,10 +754,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>11</v>
@@ -762,16 +789,12 @@
       <c r="P2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="V2" s="2"/>
       <c r="W2" s="2" t="s">
         <v>14</v>
       </c>
@@ -816,11 +839,11 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
-        <v>1657</v>
-      </c>
-      <c r="F3" s="2">
-        <v>17</v>
+      <c r="E3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>11</v>
@@ -852,16 +875,12 @@
       <c r="P3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="V3" s="2"/>
       <c r="W3" s="2" t="s">
         <v>14</v>
       </c>
@@ -906,11 +925,11 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2">
-        <v>18</v>
+      <c r="E4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>11</v>
@@ -996,11 +1015,11 @@
       <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="2">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2">
-        <v>19</v>
+      <c r="E5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>11</v>
@@ -1086,11 +1105,11 @@
       <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="E6" s="2">
-        <v>12</v>
-      </c>
-      <c r="F6" s="2">
-        <v>20</v>
+      <c r="E6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>11</v>
@@ -1176,11 +1195,11 @@
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="2">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2">
-        <v>21</v>
+      <c r="E7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>11</v>

</xml_diff>